<commit_message>
Add: new example for complete assessment by using the excel data input: ".assessment_excel_data_input.R"
plus: Some functions and variables renamed, Data input check transfered to the data loading functions

not finished yet: Some Vignettes do not work with new functions
</commit_message>
<xml_diff>
--- a/inst/extdata/Data_entry/Bsp_Herne.xlsx
+++ b/inst/extdata/Data_entry/Bsp_Herne.xlsx
@@ -1,25 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20379"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\r2q\inst\extdata\Data_entry\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE2258C-70F3-48BD-9800-F238B2377DCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_data" sheetId="1" r:id="rId1"/>
-    <sheet name="surface_data" sheetId="2" r:id="rId2"/>
+    <sheet name="surface_data" sheetId="4" r:id="rId2"/>
     <sheet name="pollution_data" sheetId="3" r:id="rId3"/>
+    <sheet name="surface_data_2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="area_plan">site_data!$C$24</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="118">
   <si>
     <t>Parameter</t>
   </si>
@@ -378,7 +385,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -789,6 +796,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1080,22 +1090,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.26953125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1125,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="56" t="s">
         <v>107</v>
       </c>
@@ -1125,7 +1135,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="41" t="s">
         <v>114</v>
       </c>
@@ -1139,7 +1149,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="41" t="s">
         <v>109</v>
       </c>
@@ -1155,7 +1165,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="41" t="s">
         <v>110</v>
       </c>
@@ -1171,7 +1181,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="47" t="s">
         <v>46</v>
       </c>
@@ -1180,7 +1190,7 @@
       <c r="D6" s="49"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
@@ -1193,7 +1203,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
@@ -1206,7 +1216,7 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>9</v>
       </c>
@@ -1219,7 +1229,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>11</v>
       </c>
@@ -1237,7 +1247,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>14</v>
       </c>
@@ -1255,7 +1265,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>17</v>
       </c>
@@ -1273,7 +1283,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
         <v>21</v>
       </c>
@@ -1291,7 +1301,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>31</v>
       </c>
@@ -1309,7 +1319,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="50" t="s">
         <v>50</v>
       </c>
@@ -1318,7 +1328,7 @@
       <c r="D15" s="52"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>23</v>
       </c>
@@ -1336,7 +1346,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>56</v>
       </c>
@@ -1354,7 +1364,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>29</v>
       </c>
@@ -1372,7 +1382,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>54</v>
       </c>
@@ -1390,7 +1400,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>55</v>
       </c>
@@ -1406,7 +1416,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
         <v>52</v>
       </c>
@@ -1424,7 +1434,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
         <v>53</v>
       </c>
@@ -1440,7 +1450,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="53" t="s">
         <v>49</v>
       </c>
@@ -1450,7 +1460,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="33" t="s">
         <v>36</v>
       </c>
@@ -1458,7 +1468,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="39">
-        <v>1</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="D24" s="37" t="s">
         <v>37</v>
@@ -1468,7 +1478,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="33" t="s">
         <v>57</v>
       </c>
@@ -1486,7 +1496,7 @@
       </c>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="35" t="s">
         <v>30</v>
       </c>
@@ -1515,22 +1525,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A50F2BF8-68DC-4187-BCB7-570F73CF5435}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>60</v>
       </c>
@@ -1547,140 +1551,36 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="24"/>
       <c r="B2" s="23" t="s">
         <v>104</v>
       </c>
       <c r="C2" s="23">
         <f>area_plan*100</f>
-        <v>100</v>
+        <v>9.6</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
       <c r="B4" t="s">
         <v>66</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="E4">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7">
-        <v>0.4</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8">
-        <v>0.1</v>
-      </c>
-      <c r="E8">
         <v>0.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9">
-        <v>0.1</v>
-      </c>
-      <c r="E9">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10">
-        <v>0.1</v>
-      </c>
-      <c r="E10">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11">
-        <v>0.1</v>
-      </c>
-      <c r="E11">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12">
-        <v>0.1</v>
-      </c>
-      <c r="E12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13">
-        <v>0.1</v>
-      </c>
-      <c r="E13">
-        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -1689,22 +1589,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
         <v>117</v>
       </c>
@@ -1718,7 +1618,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>75</v>
       </c>
@@ -1732,7 +1632,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>78</v>
       </c>
@@ -1746,7 +1646,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>80</v>
       </c>
@@ -1760,7 +1660,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>83</v>
       </c>
@@ -1774,7 +1674,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>84</v>
       </c>
@@ -1788,7 +1688,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>85</v>
       </c>
@@ -1802,7 +1702,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>87</v>
       </c>
@@ -1816,7 +1716,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>88</v>
       </c>
@@ -1830,7 +1730,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>89</v>
       </c>
@@ -1844,7 +1744,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>90</v>
       </c>
@@ -1858,7 +1758,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>91</v>
       </c>
@@ -1872,7 +1772,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>92</v>
       </c>
@@ -1886,7 +1786,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>93</v>
       </c>
@@ -1900,7 +1800,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>94</v>
       </c>
@@ -1914,7 +1814,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
         <v>95</v>
       </c>
@@ -1928,7 +1828,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
         <v>96</v>
       </c>
@@ -1942,7 +1842,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
         <v>97</v>
       </c>
@@ -1956,7 +1856,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>98</v>
       </c>
@@ -1970,7 +1870,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
         <v>99</v>
       </c>
@@ -1984,7 +1884,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
         <v>101</v>
       </c>
@@ -1998,7 +1898,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>103</v>
       </c>
@@ -2016,4 +1916,178 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="34.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="24"/>
+      <c r="B2" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="23">
+        <f>area_plan*100</f>
+        <v>9.6</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11"/>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="11"/>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="11"/>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7">
+        <v>0.4</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="11"/>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+      <c r="E8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="11"/>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="11"/>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
+      <c r="E11">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="11"/>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="11"/>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="E13">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>